<commit_message>
Added Exception + Modified code to print a message when a word is not found * Add an exception in the list of Queried Words (in puzzle.xlsx)
</commit_message>
<xml_diff>
--- a/puzzle.xlsx
+++ b/puzzle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEVELOPMENT\Python\Word Puzzle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEVELOPMENT\Python\GITHUB\Word-Search-Puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0724B76A-C584-49A5-8BC7-B564965410D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD01D32E-C469-447C-84B1-0D9093FC396E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B33AE50D-7B22-4185-9501-75B76830D4D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B33AE50D-7B22-4185-9501-75B76830D4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Puzzle" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="76">
   <si>
     <t>A</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>ONLY YOU</t>
+  </si>
+  <si>
+    <t>NOTHING</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A606266A-DCEE-494C-BF23-178DB9C600DC}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
@@ -1869,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23112D4D-DFEE-4871-9C29-DF268EC873E4}">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,191 +1940,196 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>